<commit_message>
Add more calibration and new offset
</commit_message>
<xml_diff>
--- a/code/calib.xlsx
+++ b/code/calib.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="18300" yWindow="2560" windowWidth="20320" windowHeight="17620" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="38400" windowHeight="21080" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <connection id="1" name="calibration_office" type="6" refreshedVersion="0" background="1">
-    <textPr fileType="mac" codePage="10000" sourceFile="/Users/mnapp/Documents/mydata/software/markus-napp.de/code/calibration_office.csv" thousands="." tab="0" comma="1">
+    <textPr fileType="mac" sourceFile="/Users/mnapp/Documents/mydata/software/markus-napp.de/code/calibration_office.csv" thousands="." tab="0" comma="1">
       <textFields count="4">
         <textField/>
         <textField/>
@@ -43,7 +43,7 @@
     </textPr>
   </connection>
   <connection id="2" name="calibration_office1" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" sourceFile="/Users/mnapp/Documents/mydata/software/markus-napp.de/code/calibration_office.csv" tab="0" comma="1">
+    <textPr fileType="mac" sourceFile="/Users/mnapp/Documents/mydata/software/markus-napp.de/code/calibration_office.csv" tab="0" comma="1">
       <textFields count="4">
         <textField/>
         <textField/>
@@ -391,10 +391,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:H44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+      <selection activeCell="J37" sqref="J37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -931,6 +931,67 @@
         <v>0.88246184706666675</v>
       </c>
     </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H28" s="3">
+        <v>0.81766399999999995</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H29" s="3">
+        <v>0.98443800000000004</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H30" s="3">
+        <v>0.81528100000000003</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H31" s="3">
+        <v>0.88751100000000005</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H32" s="3">
+        <v>0.78368800000000005</v>
+      </c>
+    </row>
+    <row r="33" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H33" s="3">
+        <v>0.76649500000000004</v>
+      </c>
+    </row>
+    <row r="34" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H34" s="3">
+        <v>0.88601600000000003</v>
+      </c>
+    </row>
+    <row r="35" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H35" s="3">
+        <v>0.86872000000000005</v>
+      </c>
+    </row>
+    <row r="36" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H36" s="3">
+        <v>0.86872000000000005</v>
+      </c>
+    </row>
+    <row r="37" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H37" s="3">
+        <v>1.0224899999999999</v>
+      </c>
+    </row>
+    <row r="38" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H38" s="3">
+        <v>0.84937700000000005</v>
+      </c>
+    </row>
+    <row r="44" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H44">
+        <f>AVERAGE(H28:H43)</f>
+        <v>0.86821818181818178</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>